<commit_message>
Add test manifest, template mapping and mark calculation
</commit_message>
<xml_diff>
--- a/pyam/template-template.xlsx
+++ b/pyam/template-template.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Assessment" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Scoring" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="descriptors" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Changes" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -22,8 +22,8 @@
     <definedName function="false" hidden="false" name="date" vbProcedure="false">Assessment!$B$10</definedName>
     <definedName function="false" hidden="false" name="institution_department" vbProcedure="false">Assessment!$A$1</definedName>
     <definedName function="false" hidden="false" name="mark" vbProcedure="false">Assessment!$B$11</definedName>
-    <definedName function="false" hidden="false" name="scoring" vbProcedure="false">Scoring!$A$2:$B$7</definedName>
-    <definedName function="false" hidden="false" name="scoring_text" vbProcedure="false">Scoring!$A$2:$A$7</definedName>
+    <definedName function="false" hidden="false" name="scoring" vbProcedure="false">descriptors!$A$2:$B$9</definedName>
+    <definedName function="false" hidden="false" name="scoring_text" vbProcedure="false">descriptors!$A$2:$A$9</definedName>
     <definedName function="false" hidden="false" name="student_course" vbProcedure="false">Assessment!$B$7</definedName>
     <definedName function="false" hidden="false" name="student_email" vbProcedure="false">Assessment!$B$6</definedName>
     <definedName function="false" hidden="false" name="student_id" vbProcedure="false">Assessment!$B$5</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="56">
   <si>
     <t xml:space="preserve">Institution Department</t>
   </si>
@@ -78,6 +78,12 @@
     <t xml:space="preserve">Test Results</t>
   </si>
   <si>
+    <t xml:space="preserve">Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test start here</t>
   </si>
   <si>
@@ -90,25 +96,49 @@
     <t xml:space="preserve">Score</t>
   </si>
   <si>
+    <t xml:space="preserve">Failed Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not Present</t>
   </si>
   <si>
+    <t xml:space="preserve">Invalid or missing aspect</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inadequate</t>
   </si>
   <si>
+    <t xml:space="preserve">Submission does not meet minimum requirements</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adequate</t>
   </si>
   <si>
+    <t xml:space="preserve">Meets pass thresold but does not meet all specifications</t>
+  </si>
+  <si>
     <t xml:space="preserve">Good</t>
   </si>
   <si>
+    <t xml:space="preserve">Meets specifications but may not be properly justified or explained.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Excellent</t>
   </si>
   <si>
+    <t xml:space="preserve">Meets specifications and is justified or explained.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Outstanding</t>
   </si>
   <si>
+    <t xml:space="preserve">Exceeds specification and has a full justification or explaination</t>
+  </si>
+  <si>
     <t xml:space="preserve">PASSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passed Test</t>
   </si>
   <si>
     <t xml:space="preserve">Owner</t>
@@ -189,7 +219,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -275,6 +305,14 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Bitstream Vera Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
@@ -405,7 +443,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -522,11 +560,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,7 +580,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -542,12 +588,8 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -558,6 +600,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -566,11 +612,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,13 +732,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q72"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.22"/>
@@ -836,7 +882,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="24" t="n">
-        <f aca="false">100*COUNTIF(C14:C99,"PASSED")/COUNTA(C14:C99)</f>
+        <f aca="false">100*SUM(F14:F99)/SUM(D14:D99)</f>
         <v>0</v>
       </c>
       <c r="E11" s="1"/>
@@ -868,214 +914,1516 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="25"/>
     </row>
-    <row r="13" s="32" customFormat="true" ht="20.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="34" customFormat="true" ht="20.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="27"/>
       <c r="B13" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+      <c r="D13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
       <c r="P13" s="28"/>
-      <c r="Q13" s="31"/>
+      <c r="Q13" s="33"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">VLOOKUP(C14,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <f aca="false">D14*E14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34"/>
-      <c r="C15" s="33"/>
-      <c r="E15" s="35"/>
+      <c r="A15" s="36"/>
+      <c r="C15" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">VLOOKUP(C15,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <f aca="false">D15*E15</f>
+        <v>0</v>
+      </c>
       <c r="H15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C16" s="33"/>
+      <c r="C16" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">VLOOKUP(C16,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <f aca="false">D16*E16</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C17" s="33"/>
+      <c r="C17" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">VLOOKUP(C17,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <f aca="false">D17*E17</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C18" s="33"/>
+      <c r="C18" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">VLOOKUP(C18,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <f aca="false">D18*E18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C19" s="33"/>
+      <c r="C19" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">VLOOKUP(C19,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <f aca="false">D19*E19</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C20" s="33"/>
+      <c r="C20" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">VLOOKUP(C20,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <f aca="false">D20*E20</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C21" s="33"/>
+      <c r="C21" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">VLOOKUP(C21,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <f aca="false">D21*E21</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C22" s="33"/>
+      <c r="C22" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">VLOOKUP(C22,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <f aca="false">D22*E22</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C23" s="33"/>
+      <c r="C23" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">VLOOKUP(C23,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <f aca="false">D23*E23</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C24" s="33"/>
+      <c r="C24" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">VLOOKUP(C24,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <f aca="false">D24*E24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C25" s="33"/>
+      <c r="C25" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">VLOOKUP(C25,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <f aca="false">D25*E25</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C26" s="33"/>
+      <c r="C26" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">VLOOKUP(C26,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <f aca="false">D26*E26</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C27" s="33"/>
+      <c r="C27" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <f aca="false">VLOOKUP(C27,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <f aca="false">D27*E27</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C28" s="33"/>
+      <c r="C28" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">VLOOKUP(C28,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <f aca="false">D28*E28</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C29" s="33"/>
+      <c r="C29" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">VLOOKUP(C29,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <f aca="false">D29*E29</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C30" s="33"/>
+      <c r="C30" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">VLOOKUP(C30,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <f aca="false">D30*E30</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C31" s="33"/>
+      <c r="C31" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <f aca="false">VLOOKUP(C31,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <f aca="false">D31*E31</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C32" s="33"/>
+      <c r="C32" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <f aca="false">VLOOKUP(C32,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <f aca="false">D32*E32</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C33" s="33"/>
+      <c r="C33" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <f aca="false">VLOOKUP(C33,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <f aca="false">D33*E33</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C34" s="33"/>
+      <c r="C34" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">VLOOKUP(C34,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <f aca="false">D34*E34</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C35" s="33"/>
+      <c r="C35" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="false">VLOOKUP(C35,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <f aca="false">D35*E35</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C36" s="33"/>
+      <c r="C36" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <f aca="false">VLOOKUP(C36,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <f aca="false">D36*E36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C37" s="33"/>
+      <c r="C37" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <f aca="false">VLOOKUP(C37,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <f aca="false">D37*E37</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C38" s="33"/>
+      <c r="C38" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">VLOOKUP(C38,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <f aca="false">D38*E38</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C39" s="33"/>
+      <c r="C39" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">VLOOKUP(C39,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <f aca="false">D39*E39</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="33"/>
+      <c r="C40" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">VLOOKUP(C40,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <f aca="false">D40*E40</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="33"/>
+      <c r="C41" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <f aca="false">VLOOKUP(C41,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <f aca="false">D41*E41</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="33"/>
+      <c r="C42" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">VLOOKUP(C42,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <f aca="false">D42*E42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="33"/>
+      <c r="C43" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">VLOOKUP(C43,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <f aca="false">D43*E43</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C44" s="33"/>
+      <c r="C44" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">VLOOKUP(C44,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <f aca="false">D44*E44</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="33"/>
+      <c r="C45" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">VLOOKUP(C45,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <f aca="false">D45*E45</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="33"/>
+      <c r="C46" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">VLOOKUP(C46,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <f aca="false">D46*E46</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="33"/>
+      <c r="C47" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">VLOOKUP(C47,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="2" t="n">
+        <f aca="false">D47*E47</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="33"/>
+      <c r="C48" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">VLOOKUP(C48,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="2" t="n">
+        <f aca="false">D48*E48</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="33"/>
+      <c r="C49" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">VLOOKUP(C49,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <f aca="false">D49*E49</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="33"/>
+      <c r="C50" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <f aca="false">VLOOKUP(C50,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="2" t="n">
+        <f aca="false">D50*E50</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="33"/>
+      <c r="C51" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <f aca="false">VLOOKUP(C51,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <f aca="false">D51*E51</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="33"/>
+      <c r="C52" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <f aca="false">VLOOKUP(C52,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="2" t="n">
+        <f aca="false">D52*E52</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="33"/>
+      <c r="C53" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <f aca="false">VLOOKUP(C53,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="2" t="n">
+        <f aca="false">D53*E53</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="33"/>
+      <c r="C54" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">VLOOKUP(C54,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="2" t="n">
+        <f aca="false">D54*E54</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="33"/>
+      <c r="C55" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <f aca="false">VLOOKUP(C55,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="2" t="n">
+        <f aca="false">D55*E55</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="33"/>
+      <c r="C56" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <f aca="false">VLOOKUP(C56,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <f aca="false">D56*E56</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="33"/>
+      <c r="C57" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">VLOOKUP(C57,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <f aca="false">D57*E57</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="33"/>
+      <c r="C58" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <f aca="false">VLOOKUP(C58,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <f aca="false">D58*E58</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="33"/>
+      <c r="C59" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <f aca="false">VLOOKUP(C59,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="2" t="n">
+        <f aca="false">D59*E59</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="33"/>
+      <c r="C60" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <f aca="false">VLOOKUP(C60,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="2" t="n">
+        <f aca="false">D60*E60</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="33"/>
+      <c r="C61" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <f aca="false">VLOOKUP(C61,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="2" t="n">
+        <f aca="false">D61*E61</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="33"/>
+      <c r="C62" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <f aca="false">VLOOKUP(C62,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="2" t="n">
+        <f aca="false">D62*E62</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="33"/>
+      <c r="C63" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <f aca="false">VLOOKUP(C63,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="2" t="n">
+        <f aca="false">D63*E63</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="33"/>
+      <c r="C64" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <f aca="false">VLOOKUP(C64,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F64" s="2" t="n">
+        <f aca="false">D64*E64</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="33"/>
+      <c r="C65" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <f aca="false">VLOOKUP(C65,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F65" s="2" t="n">
+        <f aca="false">D65*E65</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="33"/>
+      <c r="C66" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <f aca="false">VLOOKUP(C66,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="2" t="n">
+        <f aca="false">D66*E66</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="33"/>
+      <c r="C67" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <f aca="false">VLOOKUP(C67,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="n">
+        <f aca="false">D67*E67</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C68" s="33"/>
+      <c r="C68" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <f aca="false">VLOOKUP(C68,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F68" s="2" t="n">
+        <f aca="false">D68*E68</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C69" s="33"/>
+      <c r="C69" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <f aca="false">VLOOKUP(C69,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="2" t="n">
+        <f aca="false">D69*E69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C70" s="33"/>
+      <c r="C70" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <f aca="false">VLOOKUP(C70,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <f aca="false">D70*E70</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="33"/>
+      <c r="C71" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <f aca="false">VLOOKUP(C71,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F71" s="2" t="n">
+        <f aca="false">D71*E71</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C72" s="33"/>
-    </row>
+      <c r="C72" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <f aca="false">VLOOKUP(C72,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="n">
+        <f aca="false">D72*E72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <f aca="false">VLOOKUP(C73,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="n">
+        <f aca="false">D73*E73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <f aca="false">VLOOKUP(C74,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F74" s="2" t="n">
+        <f aca="false">D74*E74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C75" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <f aca="false">VLOOKUP(C75,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="n">
+        <f aca="false">D75*E75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C76" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <f aca="false">VLOOKUP(C76,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F76" s="2" t="n">
+        <f aca="false">D76*E76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <f aca="false">VLOOKUP(C77,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F77" s="2" t="n">
+        <f aca="false">D77*E77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <f aca="false">VLOOKUP(C78,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F78" s="2" t="n">
+        <f aca="false">D78*E78</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <f aca="false">VLOOKUP(C79,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="n">
+        <f aca="false">D79*E79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <f aca="false">VLOOKUP(C80,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="n">
+        <f aca="false">D80*E80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <f aca="false">VLOOKUP(C81,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F81" s="2" t="n">
+        <f aca="false">D81*E81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <f aca="false">VLOOKUP(C82,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="n">
+        <f aca="false">D82*E82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <f aca="false">VLOOKUP(C83,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F83" s="2" t="n">
+        <f aca="false">D83*E83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <f aca="false">VLOOKUP(C84,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="n">
+        <f aca="false">D84*E84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C85" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <f aca="false">VLOOKUP(C85,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="n">
+        <f aca="false">D85*E85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <f aca="false">VLOOKUP(C86,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F86" s="2" t="n">
+        <f aca="false">D86*E86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <f aca="false">VLOOKUP(C87,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="n">
+        <f aca="false">D87*E87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <f aca="false">VLOOKUP(C88,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F88" s="2" t="n">
+        <f aca="false">D88*E88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <f aca="false">VLOOKUP(C89,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="n">
+        <f aca="false">D89*E89</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <f aca="false">VLOOKUP(C90,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F90" s="2" t="n">
+        <f aca="false">D90*E90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <f aca="false">VLOOKUP(C91,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F91" s="2" t="n">
+        <f aca="false">D91*E91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <f aca="false">VLOOKUP(C92,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F92" s="2" t="n">
+        <f aca="false">D92*E92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <f aca="false">VLOOKUP(C93,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F93" s="2" t="n">
+        <f aca="false">D93*E93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <f aca="false">VLOOKUP(C94,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F94" s="2" t="n">
+        <f aca="false">D94*E94</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <f aca="false">VLOOKUP(C95,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F95" s="2" t="n">
+        <f aca="false">D95*E95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <f aca="false">VLOOKUP(C96,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F96" s="2" t="n">
+        <f aca="false">D96*E96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <f aca="false">VLOOKUP(C97,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F97" s="2" t="n">
+        <f aca="false">D97*E97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C98" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <f aca="false">VLOOKUP(C98,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F98" s="2" t="n">
+        <f aca="false">D98*E98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C99" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <f aca="false">VLOOKUP(C99,scoring,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F99" s="2" t="n">
+        <f aca="false">D99*E99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="C14:C72">
+  <conditionalFormatting sqref="C14:C99">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"FAILED"</formula>
     </cfRule>
@@ -1083,27 +2431,23 @@
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B6" type="none">
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B6" type="none">
       <formula1>#name?</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E15" type="list">
-      <formula1>scoring_text</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B2 B10" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B2 B10" type="none">
       <formula1>2020/1/1</formula1>
       <formula2>2020/12/31</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C14:C100" type="list">
-      <formula1>"PASSED,FAILED"</formula1>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C14:C99" type="list">
+      <formula1>scoring_text</formula1>
       <formula2>2020/12/31</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1116,111 +2460,140 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="59.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="37" width="59.89"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="37"/>
+        <v>17</v>
+      </c>
+      <c r="C1" s="38"/>
     </row>
     <row r="2" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
+      <c r="A2" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>2</v>
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>3</v>
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>4</v>
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B9" s="17" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" s="36" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="38"/>
-    </row>
-    <row r="11" s="36" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="38"/>
-    </row>
-    <row r="12" s="36" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="38"/>
-    </row>
-    <row r="13" s="36" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="38"/>
-    </row>
-    <row r="14" s="36" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="38"/>
-    </row>
-    <row r="15" s="36" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="38"/>
+      <c r="C9" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" s="37" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="40"/>
+    </row>
+    <row r="13" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="40"/>
+    </row>
+    <row r="14" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="40"/>
+    </row>
+    <row r="15" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="40"/>
+    </row>
+    <row r="16" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="40"/>
+    </row>
+    <row r="17" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="40"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1239,118 +2612,118 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="91.56"/>
   </cols>
   <sheetData>
-    <row r="1" s="41" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+    <row r="1" s="43" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>27</v>
+      <c r="B1" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="n">
+      <c r="A2" s="41" t="n">
         <v>44014</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="n">
+      <c r="A3" s="41" t="n">
         <v>44015</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="n">
+      <c r="A4" s="41" t="n">
         <v>44018</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add "cell" attribute to test data
</commit_message>
<xml_diff>
--- a/pyam/template-template.xlsx
+++ b/pyam/template-template.xlsx
@@ -22,8 +22,8 @@
     <definedName function="false" hidden="false" name="date" vbProcedure="false">Assessment!$B$10</definedName>
     <definedName function="false" hidden="false" name="institution_department" vbProcedure="false">Assessment!$A$1</definedName>
     <definedName function="false" hidden="false" name="mark" vbProcedure="false">Assessment!$B$11</definedName>
-    <definedName function="false" hidden="false" name="scoring" vbProcedure="false">descriptors!$A$2:$B$9</definedName>
-    <definedName function="false" hidden="false" name="scoring_text" vbProcedure="false">descriptors!$A$2:$A$9</definedName>
+    <definedName function="false" hidden="false" name="scoring" vbProcedure="false">descriptors!$A$2:$B$12</definedName>
+    <definedName function="false" hidden="false" name="scoring_text" vbProcedure="false">descriptors!$A$2:$A$12</definedName>
     <definedName function="false" hidden="false" name="student_course" vbProcedure="false">Assessment!$B$7</definedName>
     <definedName function="false" hidden="false" name="student_email" vbProcedure="false">Assessment!$B$6</definedName>
     <definedName function="false" hidden="false" name="student_id" vbProcedure="false">Assessment!$B$5</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
   <si>
     <t xml:space="preserve">Institution Department</t>
   </si>
@@ -99,6 +99,12 @@
     <t xml:space="preserve">Failed Test</t>
   </si>
   <si>
+    <t xml:space="preserve">Incorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item is incorrect</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not Present</t>
   </si>
   <si>
@@ -133,6 +139,18 @@
   </si>
   <si>
     <t xml:space="preserve">Exceeds specification and has a full justification or explaination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item is correct</t>
   </si>
   <si>
     <t xml:space="preserve">PASSED</t>
@@ -734,11 +752,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.22"/>
@@ -950,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="0" t="n">
-        <f aca="false">VLOOKUP(C14,scoring,2)</f>
+        <f aca="false">VLOOKUP(C14,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F14" s="2" t="n">
@@ -967,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="0" t="n">
-        <f aca="false">VLOOKUP(C15,scoring,2)</f>
+        <f aca="false">VLOOKUP(C15,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
@@ -984,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="0" t="n">
-        <f aca="false">VLOOKUP(C16,scoring,2)</f>
+        <f aca="false">VLOOKUP(C16,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
@@ -1000,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="0" t="n">
-        <f aca="false">VLOOKUP(C17,scoring,2)</f>
+        <f aca="false">VLOOKUP(C17,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
@@ -1016,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="0" t="n">
-        <f aca="false">VLOOKUP(C18,scoring,2)</f>
+        <f aca="false">VLOOKUP(C18,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
@@ -1032,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="0" t="n">
-        <f aca="false">VLOOKUP(C19,scoring,2)</f>
+        <f aca="false">VLOOKUP(C19,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
@@ -1048,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="0" t="n">
-        <f aca="false">VLOOKUP(C20,scoring,2)</f>
+        <f aca="false">VLOOKUP(C20,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
@@ -1064,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="0" t="n">
-        <f aca="false">VLOOKUP(C21,scoring,2)</f>
+        <f aca="false">VLOOKUP(C21,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
@@ -1080,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="0" t="n">
-        <f aca="false">VLOOKUP(C22,scoring,2)</f>
+        <f aca="false">VLOOKUP(C22,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F22" s="2" t="n">
@@ -1096,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="0" t="n">
-        <f aca="false">VLOOKUP(C23,scoring,2)</f>
+        <f aca="false">VLOOKUP(C23,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F23" s="2" t="n">
@@ -1112,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="0" t="n">
-        <f aca="false">VLOOKUP(C24,scoring,2)</f>
+        <f aca="false">VLOOKUP(C24,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F24" s="2" t="n">
@@ -1128,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="0" t="n">
-        <f aca="false">VLOOKUP(C25,scoring,2)</f>
+        <f aca="false">VLOOKUP(C25,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F25" s="2" t="n">
@@ -1144,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="0" t="n">
-        <f aca="false">VLOOKUP(C26,scoring,2)</f>
+        <f aca="false">VLOOKUP(C26,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F26" s="2" t="n">
@@ -1160,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="0" t="n">
-        <f aca="false">VLOOKUP(C27,scoring,2)</f>
+        <f aca="false">VLOOKUP(C27,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F27" s="2" t="n">
@@ -1176,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="0" t="n">
-        <f aca="false">VLOOKUP(C28,scoring,2)</f>
+        <f aca="false">VLOOKUP(C28,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F28" s="2" t="n">
@@ -1192,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="0" t="n">
-        <f aca="false">VLOOKUP(C29,scoring,2)</f>
+        <f aca="false">VLOOKUP(C29,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F29" s="2" t="n">
@@ -1208,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="0" t="n">
-        <f aca="false">VLOOKUP(C30,scoring,2)</f>
+        <f aca="false">VLOOKUP(C30,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F30" s="2" t="n">
@@ -1224,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="0" t="n">
-        <f aca="false">VLOOKUP(C31,scoring,2)</f>
+        <f aca="false">VLOOKUP(C31,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F31" s="2" t="n">
@@ -1240,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="0" t="n">
-        <f aca="false">VLOOKUP(C32,scoring,2)</f>
+        <f aca="false">VLOOKUP(C32,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F32" s="2" t="n">
@@ -1256,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="0" t="n">
-        <f aca="false">VLOOKUP(C33,scoring,2)</f>
+        <f aca="false">VLOOKUP(C33,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F33" s="2" t="n">
@@ -1272,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="0" t="n">
-        <f aca="false">VLOOKUP(C34,scoring,2)</f>
+        <f aca="false">VLOOKUP(C34,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F34" s="2" t="n">
@@ -1288,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="0" t="n">
-        <f aca="false">VLOOKUP(C35,scoring,2)</f>
+        <f aca="false">VLOOKUP(C35,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F35" s="2" t="n">
@@ -1304,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="0" t="n">
-        <f aca="false">VLOOKUP(C36,scoring,2)</f>
+        <f aca="false">VLOOKUP(C36,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F36" s="2" t="n">
@@ -1320,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="0" t="n">
-        <f aca="false">VLOOKUP(C37,scoring,2)</f>
+        <f aca="false">VLOOKUP(C37,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F37" s="2" t="n">
@@ -1336,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="0" t="n">
-        <f aca="false">VLOOKUP(C38,scoring,2)</f>
+        <f aca="false">VLOOKUP(C38,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
@@ -1352,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="0" t="n">
-        <f aca="false">VLOOKUP(C39,scoring,2)</f>
+        <f aca="false">VLOOKUP(C39,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F39" s="2" t="n">
@@ -1368,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="0" t="n">
-        <f aca="false">VLOOKUP(C40,scoring,2)</f>
+        <f aca="false">VLOOKUP(C40,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
@@ -1384,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="0" t="n">
-        <f aca="false">VLOOKUP(C41,scoring,2)</f>
+        <f aca="false">VLOOKUP(C41,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
@@ -1400,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="0" t="n">
-        <f aca="false">VLOOKUP(C42,scoring,2)</f>
+        <f aca="false">VLOOKUP(C42,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
@@ -1416,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="0" t="n">
-        <f aca="false">VLOOKUP(C43,scoring,2)</f>
+        <f aca="false">VLOOKUP(C43,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F43" s="2" t="n">
@@ -1432,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="0" t="n">
-        <f aca="false">VLOOKUP(C44,scoring,2)</f>
+        <f aca="false">VLOOKUP(C44,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F44" s="2" t="n">
@@ -1448,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="0" t="n">
-        <f aca="false">VLOOKUP(C45,scoring,2)</f>
+        <f aca="false">VLOOKUP(C45,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F45" s="2" t="n">
@@ -1464,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="0" t="n">
-        <f aca="false">VLOOKUP(C46,scoring,2)</f>
+        <f aca="false">VLOOKUP(C46,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F46" s="2" t="n">
@@ -1480,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="0" t="n">
-        <f aca="false">VLOOKUP(C47,scoring,2)</f>
+        <f aca="false">VLOOKUP(C47,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F47" s="2" t="n">
@@ -1496,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="0" t="n">
-        <f aca="false">VLOOKUP(C48,scoring,2)</f>
+        <f aca="false">VLOOKUP(C48,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F48" s="2" t="n">
@@ -1512,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="0" t="n">
-        <f aca="false">VLOOKUP(C49,scoring,2)</f>
+        <f aca="false">VLOOKUP(C49,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F49" s="2" t="n">
@@ -1528,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="0" t="n">
-        <f aca="false">VLOOKUP(C50,scoring,2)</f>
+        <f aca="false">VLOOKUP(C50,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F50" s="2" t="n">
@@ -1544,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="0" t="n">
-        <f aca="false">VLOOKUP(C51,scoring,2)</f>
+        <f aca="false">VLOOKUP(C51,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F51" s="2" t="n">
@@ -1560,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="0" t="n">
-        <f aca="false">VLOOKUP(C52,scoring,2)</f>
+        <f aca="false">VLOOKUP(C52,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F52" s="2" t="n">
@@ -1576,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="0" t="n">
-        <f aca="false">VLOOKUP(C53,scoring,2)</f>
+        <f aca="false">VLOOKUP(C53,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F53" s="2" t="n">
@@ -1592,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="0" t="n">
-        <f aca="false">VLOOKUP(C54,scoring,2)</f>
+        <f aca="false">VLOOKUP(C54,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F54" s="2" t="n">
@@ -1608,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="0" t="n">
-        <f aca="false">VLOOKUP(C55,scoring,2)</f>
+        <f aca="false">VLOOKUP(C55,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F55" s="2" t="n">
@@ -1624,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="0" t="n">
-        <f aca="false">VLOOKUP(C56,scoring,2)</f>
+        <f aca="false">VLOOKUP(C56,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F56" s="2" t="n">
@@ -1640,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="0" t="n">
-        <f aca="false">VLOOKUP(C57,scoring,2)</f>
+        <f aca="false">VLOOKUP(C57,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F57" s="2" t="n">
@@ -1656,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="0" t="n">
-        <f aca="false">VLOOKUP(C58,scoring,2)</f>
+        <f aca="false">VLOOKUP(C58,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F58" s="2" t="n">
@@ -1672,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="0" t="n">
-        <f aca="false">VLOOKUP(C59,scoring,2)</f>
+        <f aca="false">VLOOKUP(C59,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F59" s="2" t="n">
@@ -1688,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="0" t="n">
-        <f aca="false">VLOOKUP(C60,scoring,2)</f>
+        <f aca="false">VLOOKUP(C60,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F60" s="2" t="n">
@@ -1704,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="0" t="n">
-        <f aca="false">VLOOKUP(C61,scoring,2)</f>
+        <f aca="false">VLOOKUP(C61,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F61" s="2" t="n">
@@ -1720,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="0" t="n">
-        <f aca="false">VLOOKUP(C62,scoring,2)</f>
+        <f aca="false">VLOOKUP(C62,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F62" s="2" t="n">
@@ -1736,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="0" t="n">
-        <f aca="false">VLOOKUP(C63,scoring,2)</f>
+        <f aca="false">VLOOKUP(C63,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F63" s="2" t="n">
@@ -1752,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="0" t="n">
-        <f aca="false">VLOOKUP(C64,scoring,2)</f>
+        <f aca="false">VLOOKUP(C64,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F64" s="2" t="n">
@@ -1768,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="E65" s="0" t="n">
-        <f aca="false">VLOOKUP(C65,scoring,2)</f>
+        <f aca="false">VLOOKUP(C65,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F65" s="2" t="n">
@@ -1784,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="E66" s="0" t="n">
-        <f aca="false">VLOOKUP(C66,scoring,2)</f>
+        <f aca="false">VLOOKUP(C66,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F66" s="2" t="n">
@@ -1800,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="E67" s="0" t="n">
-        <f aca="false">VLOOKUP(C67,scoring,2)</f>
+        <f aca="false">VLOOKUP(C67,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F67" s="2" t="n">
@@ -1816,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="E68" s="0" t="n">
-        <f aca="false">VLOOKUP(C68,scoring,2)</f>
+        <f aca="false">VLOOKUP(C68,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F68" s="2" t="n">
@@ -1832,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="0" t="n">
-        <f aca="false">VLOOKUP(C69,scoring,2)</f>
+        <f aca="false">VLOOKUP(C69,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F69" s="2" t="n">
@@ -1848,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="0" t="n">
-        <f aca="false">VLOOKUP(C70,scoring,2)</f>
+        <f aca="false">VLOOKUP(C70,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F70" s="2" t="n">
@@ -1864,7 +1882,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="0" t="n">
-        <f aca="false">VLOOKUP(C71,scoring,2)</f>
+        <f aca="false">VLOOKUP(C71,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F71" s="2" t="n">
@@ -1880,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="0" t="n">
-        <f aca="false">VLOOKUP(C72,scoring,2)</f>
+        <f aca="false">VLOOKUP(C72,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F72" s="2" t="n">
@@ -1896,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="0" t="n">
-        <f aca="false">VLOOKUP(C73,scoring,2)</f>
+        <f aca="false">VLOOKUP(C73,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F73" s="2" t="n">
@@ -1912,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="0" t="n">
-        <f aca="false">VLOOKUP(C74,scoring,2)</f>
+        <f aca="false">VLOOKUP(C74,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F74" s="2" t="n">
@@ -1928,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="E75" s="0" t="n">
-        <f aca="false">VLOOKUP(C75,scoring,2)</f>
+        <f aca="false">VLOOKUP(C75,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F75" s="2" t="n">
@@ -1944,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="0" t="n">
-        <f aca="false">VLOOKUP(C76,scoring,2)</f>
+        <f aca="false">VLOOKUP(C76,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F76" s="2" t="n">
@@ -1960,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="0" t="n">
-        <f aca="false">VLOOKUP(C77,scoring,2)</f>
+        <f aca="false">VLOOKUP(C77,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F77" s="2" t="n">
@@ -1976,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="0" t="n">
-        <f aca="false">VLOOKUP(C78,scoring,2)</f>
+        <f aca="false">VLOOKUP(C78,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F78" s="2" t="n">
@@ -1992,7 +2010,7 @@
         <v>1</v>
       </c>
       <c r="E79" s="0" t="n">
-        <f aca="false">VLOOKUP(C79,scoring,2)</f>
+        <f aca="false">VLOOKUP(C79,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F79" s="2" t="n">
@@ -2008,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="E80" s="0" t="n">
-        <f aca="false">VLOOKUP(C80,scoring,2)</f>
+        <f aca="false">VLOOKUP(C80,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F80" s="2" t="n">
@@ -2024,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="E81" s="0" t="n">
-        <f aca="false">VLOOKUP(C81,scoring,2)</f>
+        <f aca="false">VLOOKUP(C81,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F81" s="2" t="n">
@@ -2040,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="E82" s="0" t="n">
-        <f aca="false">VLOOKUP(C82,scoring,2)</f>
+        <f aca="false">VLOOKUP(C82,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F82" s="2" t="n">
@@ -2056,7 +2074,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="0" t="n">
-        <f aca="false">VLOOKUP(C83,scoring,2)</f>
+        <f aca="false">VLOOKUP(C83,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F83" s="2" t="n">
@@ -2072,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="E84" s="0" t="n">
-        <f aca="false">VLOOKUP(C84,scoring,2)</f>
+        <f aca="false">VLOOKUP(C84,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F84" s="2" t="n">
@@ -2088,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="E85" s="0" t="n">
-        <f aca="false">VLOOKUP(C85,scoring,2)</f>
+        <f aca="false">VLOOKUP(C85,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F85" s="2" t="n">
@@ -2104,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="E86" s="0" t="n">
-        <f aca="false">VLOOKUP(C86,scoring,2)</f>
+        <f aca="false">VLOOKUP(C86,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F86" s="2" t="n">
@@ -2120,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="0" t="n">
-        <f aca="false">VLOOKUP(C87,scoring,2)</f>
+        <f aca="false">VLOOKUP(C87,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F87" s="2" t="n">
@@ -2136,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="0" t="n">
-        <f aca="false">VLOOKUP(C88,scoring,2)</f>
+        <f aca="false">VLOOKUP(C88,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F88" s="2" t="n">
@@ -2152,7 +2170,7 @@
         <v>1</v>
       </c>
       <c r="E89" s="0" t="n">
-        <f aca="false">VLOOKUP(C89,scoring,2)</f>
+        <f aca="false">VLOOKUP(C89,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F89" s="2" t="n">
@@ -2168,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="E90" s="0" t="n">
-        <f aca="false">VLOOKUP(C90,scoring,2)</f>
+        <f aca="false">VLOOKUP(C90,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F90" s="2" t="n">
@@ -2184,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="E91" s="0" t="n">
-        <f aca="false">VLOOKUP(C91,scoring,2)</f>
+        <f aca="false">VLOOKUP(C91,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F91" s="2" t="n">
@@ -2200,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="0" t="n">
-        <f aca="false">VLOOKUP(C92,scoring,2)</f>
+        <f aca="false">VLOOKUP(C92,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F92" s="2" t="n">
@@ -2216,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="0" t="n">
-        <f aca="false">VLOOKUP(C93,scoring,2)</f>
+        <f aca="false">VLOOKUP(C93,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F93" s="2" t="n">
@@ -2232,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="E94" s="0" t="n">
-        <f aca="false">VLOOKUP(C94,scoring,2)</f>
+        <f aca="false">VLOOKUP(C94,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F94" s="2" t="n">
@@ -2248,7 +2266,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="0" t="n">
-        <f aca="false">VLOOKUP(C95,scoring,2)</f>
+        <f aca="false">VLOOKUP(C95,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F95" s="2" t="n">
@@ -2264,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="0" t="n">
-        <f aca="false">VLOOKUP(C96,scoring,2)</f>
+        <f aca="false">VLOOKUP(C96,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F96" s="2" t="n">
@@ -2280,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="E97" s="0" t="n">
-        <f aca="false">VLOOKUP(C97,scoring,2)</f>
+        <f aca="false">VLOOKUP(C97,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F97" s="2" t="n">
@@ -2296,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="0" t="n">
-        <f aca="false">VLOOKUP(C98,scoring,2)</f>
+        <f aca="false">VLOOKUP(C98,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F98" s="2" t="n">
@@ -2312,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="0" t="n">
-        <f aca="false">VLOOKUP(C99,scoring,2)</f>
+        <f aca="false">VLOOKUP(C99,scoring,2,0)</f>
         <v>0</v>
       </c>
       <c r="F99" s="2" t="n">
@@ -2460,13 +2478,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="37" width="59.89"/>
@@ -2493,10 +2511,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="37" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="37" t="s">
@@ -2508,7 +2526,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>22</v>
@@ -2519,7 +2537,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>24</v>
@@ -2530,7 +2548,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>26</v>
@@ -2541,9 +2559,9 @@
         <v>27</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="C7" s="39" t="s">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2552,9 +2570,9 @@
         <v>29</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="37" t="s">
+        <v>0.8</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2562,26 +2580,50 @@
       <c r="A9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="17" t="n">
+      <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" s="37" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-      <c r="C12" s="40"/>
-    </row>
-    <row r="13" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="40"/>
-    </row>
-    <row r="14" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="40"/>
-    </row>
-    <row r="15" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="37" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
       <c r="C15" s="40"/>
     </row>
     <row r="16" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,6 +2631,15 @@
     </row>
     <row r="17" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="40"/>
+    </row>
+    <row r="18" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="40"/>
+    </row>
+    <row r="19" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="40"/>
+    </row>
+    <row r="20" s="37" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="40"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2612,9 +2663,9 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="91.56"/>
   </cols>
   <sheetData>
@@ -2623,19 +2674,19 @@
         <v>9</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F1" s="43" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,19 +2694,19 @@
         <v>44014</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,19 +2714,19 @@
         <v>44015</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2683,41 +2734,41 @@
         <v>44018</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>